<commit_message>
2025-07-08 Added Kanji Images for n4
</commit_message>
<xml_diff>
--- a/public/docs/kanji_n4.xlsx
+++ b/public/docs/kanji_n4.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Kanji</t>
   </si>
@@ -30,97 +30,147 @@
     <t>English</t>
   </si>
   <si>
+    <t>たび</t>
+  </si>
+  <si>
+    <t>trip</t>
+  </si>
+  <si>
+    <t>べん</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>つよい</t>
+  </si>
+  <si>
+    <t>strong</t>
+  </si>
+  <si>
+    <t>おしえる</t>
+  </si>
+  <si>
+    <t>teach</t>
+  </si>
+  <si>
+    <t>しつ</t>
+  </si>
+  <si>
+    <t>room</t>
+  </si>
+  <si>
+    <t>かい</t>
+  </si>
+  <si>
+    <t>meeting</t>
+  </si>
+  <si>
+    <t>しゃ</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>いん</t>
+  </si>
+  <si>
+    <t>member</t>
+  </si>
+  <si>
+    <t>あける</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>しめる</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>ImageName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>旅</t>
-  </si>
-  <si>
-    <t>たび</t>
-  </si>
-  <si>
-    <t>trip</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n4_trip.jpeg</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>勉</t>
-  </si>
-  <si>
-    <t>べん</t>
-  </si>
-  <si>
-    <t>study</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n4_study.jpg</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>強</t>
-  </si>
-  <si>
-    <t>つよい</t>
-  </si>
-  <si>
-    <t>strong</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n4_strong.png</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>教</t>
-  </si>
-  <si>
-    <t>おしえる</t>
-  </si>
-  <si>
-    <t>teach</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n4_teach.jpg</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>室</t>
-  </si>
-  <si>
-    <t>しつ</t>
-  </si>
-  <si>
-    <t>room</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n4_room.jpg</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>会</t>
-  </si>
-  <si>
-    <t>かい</t>
-  </si>
-  <si>
-    <t>meeting</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n4_meeting.webp</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>社</t>
-  </si>
-  <si>
-    <t>しゃ</t>
-  </si>
-  <si>
-    <t>company</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n4_company.webp</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>員</t>
-  </si>
-  <si>
-    <t>いん</t>
-  </si>
-  <si>
-    <t>member</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n4_member.jpg</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>開</t>
-  </si>
-  <si>
-    <t>あける</t>
-  </si>
-  <si>
-    <t>open</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n4_open.jpg</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>閉</t>
-  </si>
-  <si>
-    <t>しめる</t>
-  </si>
-  <si>
-    <t>close</t>
-  </si>
-  <si>
-    <t>ImageName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n4_close.webp</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -471,7 +521,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -487,121 +537,152 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="D2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+      <c r="D3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>